<commit_message>
Bug fixes, likes and comments, feed POST request
</commit_message>
<xml_diff>
--- a/Backend/custom_ds/crops.xlsx
+++ b/Backend/custom_ds/crops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taaha\OneDrive\Desktop\plant-it\Backend\custom_ds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F09E1F-CC0A-44C2-9BBF-419DC4A578EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC20E636-7659-4312-B7C4-368E08EA075C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{141E42C0-471E-4F06-9AB2-CD85BFA50CF8}"/>
   </bookViews>
@@ -155,12 +155,6 @@
     <t>rich in hums, red-loam to sandy loam, and red lateritic sandy loam</t>
   </si>
   <si>
-    <t xml:space="preserve">Cardamom </t>
-  </si>
-  <si>
-    <t>well-drained lateritic     </t>
-  </si>
-  <si>
     <t>Turmeric</t>
   </si>
   <si>
@@ -177,6 +171,12 @@
   </si>
   <si>
     <t>soil</t>
+  </si>
+  <si>
+    <t>Cardamom</t>
+  </si>
+  <si>
+    <t>well-drained lateritic</t>
   </si>
 </sst>
 </file>
@@ -557,17 +557,18 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.21875" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="58.21875" customWidth="1"/>
+    <col min="7" max="7" width="57" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="52.5546875" customWidth="1"/>
   </cols>
@@ -589,13 +590,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -622,7 +623,7 @@
         <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I2" s="3"/>
     </row>
@@ -652,7 +653,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2">
         <v>10</v>
@@ -670,7 +671,7 @@
         <v>80</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -997,7 +998,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -1015,7 +1016,7 @@
         <v>90</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>